<commit_message>
chore(docs): Update v1 and v2 of diagram  and costs
</commit_message>
<xml_diff>
--- a/docs/ADR/v2.0/ExportedEstimate.xlsx
+++ b/docs/ADR/v2.0/ExportedEstimate.xlsx
@@ -5,7 +5,7 @@
     <workbookView/>
   </bookViews>
   <sheets>
-    <sheet name="ACI" sheetId="1" r:id="rId1"/>
+    <sheet name="Your Estimate" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr fullCalcOnLoad="1"/>
 </workbook>
@@ -17,7 +17,7 @@
     <t>Microsoft Azure Estimate</t>
   </si>
   <si>
-    <t>ACI</t>
+    <t>Your Estimate</t>
   </si>
   <si>
     <t>Service category</t>
@@ -41,22 +41,37 @@
     <t>Estimated upfront cost</t>
   </si>
   <si>
+    <t>Networking</t>
+  </si>
+  <si>
+    <t>Virtual Network</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>East US 2 (Virtual Network 1): 100 GB Outbound Data Transfer; East US (Virtual Network 2): 0 GB Outbound Data Transfer</t>
+  </si>
+  <si>
+    <t>Containers</t>
+  </si>
+  <si>
+    <t>Azure Container Registry</t>
+  </si>
+  <si>
+    <t>East US 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Basic Tier, 1 registries x 30 days,   0 GB Extra Storage, Container Build - 1 CPUs x 1 Seconds - Inter Region transfer type, 5 GB outbound data transfer from East US 2 to East Asia</t>
+  </si>
+  <si>
     <t>Compute</t>
   </si>
   <si>
     <t>Azure Container Instances</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
-    <t>East US 2</t>
-  </si>
-  <si>
-    <t>1 Container group(s) x 26,28,000 Second(s), Linux OS, Pay as you go, 1 GB Memory, 1 vCPU(s)</t>
-  </si>
-  <si>
-    <t>Networking</t>
+    <t>1 Container group(s) x 2,628,000 Second(s), Linux OS, Pay as you go, 1 GB Memory, 1 vCPU(s)</t>
   </si>
   <si>
     <t>Load Balancer</t>
@@ -65,34 +80,19 @@
     <t>Standard Tier: 5 Rules, 1,000 GB Data Processed</t>
   </si>
   <si>
-    <t>Databases</t>
-  </si>
-  <si>
-    <t>Azure Cosmos DB</t>
-  </si>
-  <si>
-    <t>Azure Cosmos DB for MongoDB, Standard provisioned throughput (manual), Always-free quantity disabled, Single Region Write (Single-Master) - East US (Write Region), 400 RU/s x 730 Hours, 0 GB transactional storage, Analytical storage disabled, 2 copies of periodic backup storage</t>
-  </si>
-  <si>
-    <t>Containers</t>
-  </si>
-  <si>
-    <t>Azure Container Registry</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Basic Tier, 1 registries x 30 days,   0 GB Extra Storage, Container Build - 1 CPUs x 1 Seconds - Inter Region transfer type, 5 GB outbound data transfer from East US 2 to East Asia</t>
-  </si>
-  <si>
-    <t>Virtual Network</t>
-  </si>
-  <si>
-    <t>East US 2 (Virtual Network 1): 100 GB Outbound Data Transfer; East US 2 (Virtual Network 2): 100 GB Outbound Data Transfer</t>
-  </si>
-  <si>
     <t>IP Addresses</t>
   </si>
   <si>
     <t>Standard (ARM), 1 Static IP Addresses X 730 Hours, 0 Public IP Prefixes X 730 Hours</t>
+  </si>
+  <si>
+    <t>Storage</t>
+  </si>
+  <si>
+    <t>Storage Accounts</t>
+  </si>
+  <si>
+    <t>Block Blob Storage, General Purpose V2, Hierarchical Namespace, LRS Redundancy, Hot Access Tier, 100 GB Capacity - Pay as you go, 10 x 10,000 Write operations, 10 x 10,000 Read operations, 10 x 10,000 Iterative Read operations, 10 x 100 Iterative Write operations, 98 GB Data Retrieval, 1,000 GB Data Write, 100 GB Index, 1 x 10,000 Other operations</t>
   </si>
   <si>
     <t>Support</t>
@@ -119,7 +119,7 @@
     <t>All prices shown are in United States – Dollar ($) USD. This is a summary estimate, not a quote. For up to date pricing information please visit https://azure.microsoft.com/pricing/calculator/</t>
   </si>
   <si>
-    <t>This estimate was created at 11/21/2023 12:30:27 AM UTC.</t>
+    <t>This estimate was created at 11/24/2023 5:59:58 PM UTC.</t>
   </si>
 </sst>
 </file>
@@ -385,14 +385,12 @@
       <c r="C4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="3"/>
+      <c r="E4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>13</v>
-      </c>
       <c r="F4" s="5">
-        <v>32.8135</v>
+        <v>7</v>
       </c>
       <c r="G4" s="5">
         <v>0</v>
@@ -419,22 +417,22 @@
     </row>
     <row r="5">
       <c r="A5" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F5" s="5">
-        <v>23.25</v>
+        <v>4.998</v>
       </c>
       <c r="G5" s="5">
         <v>0</v>
@@ -470,13 +468,13 @@
         <v>11</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>19</v>
       </c>
       <c r="F6" s="5">
-        <v>23.36</v>
+        <v>32.8135</v>
       </c>
       <c r="G6" s="5">
         <v>0</v>
@@ -503,22 +501,22 @@
     </row>
     <row r="7">
       <c r="A7" s="3" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F7" s="5">
-        <v>4.998</v>
+        <v>23.25</v>
       </c>
       <c r="G7" s="5">
         <v>0</v>
@@ -545,20 +543,22 @@
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="3"/>
+      <c r="D8" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="E8" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F8" s="5">
-        <v>4</v>
+        <v>3.65</v>
       </c>
       <c r="G8" s="5">
         <v>0</v>
@@ -585,7 +585,7 @@
     </row>
     <row r="9">
       <c r="A9" s="3" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>25</v>
@@ -594,13 +594,13 @@
         <v>11</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>26</v>
       </c>
       <c r="F9" s="5">
-        <v>3.65</v>
+        <v>5.807</v>
       </c>
       <c r="G9" s="5">
         <v>0</v>
@@ -766,7 +766,7 @@
       </c>
       <c r="E14" s="12"/>
       <c r="F14" s="15">
-        <v>92.0715</v>
+        <v>77.5185</v>
       </c>
       <c r="G14" s="15">
         <v>0</v>

</xml_diff>